<commit_message>
Fin du Projet 5
</commit_message>
<xml_diff>
--- a/Plan de test fonctionnel.xlsx
+++ b/Plan de test fonctionnel.xlsx
@@ -423,6 +423,9 @@
       <c r="B2" t="str">
         <v>Affichage de la liste produit</v>
       </c>
+      <c r="C2" t="str">
+        <v>Récupération de la liste du fichier JSON, avec leur image, le nom, le prix, et le descriptif</v>
+      </c>
       <c r="D2" t="str">
         <v>Chaque articles devraient être présent avec leur image, nom, et la description</v>
       </c>
@@ -437,6 +440,9 @@
       <c r="B3" t="str">
         <v>Sélection d'un produit parmi la liste</v>
       </c>
+      <c r="C3" t="str">
+        <v>Chaque produit est cliquable et effectue une redirection de page</v>
+      </c>
       <c r="D3" t="str">
         <v>La sélection d'un article redirige l'utilisateur sur la page produit</v>
       </c>
@@ -451,6 +457,9 @@
       <c r="B4" t="str">
         <v>Affichage de la fiche produit</v>
       </c>
+      <c r="C4" t="str">
+        <v>Récupération de l'image, le nom, le prix, et le descriptif</v>
+      </c>
       <c r="D4" t="str">
         <v>L'article est présenté avec un descriptif complet, et son prix</v>
       </c>
@@ -465,11 +474,14 @@
       <c r="B5" t="str">
         <v>Sélection du coloris et de la quantité</v>
       </c>
+      <c r="C5" t="str">
+        <v>Menu déroulant pour les coloris, et input numérique pour la quantité</v>
+      </c>
       <c r="D5" t="str">
         <v>Choix des coloris disponibles de l'article, et un champ numérique indiquant la quantitié voulue</v>
       </c>
       <c r="E5" t="str">
-        <v>OK / Si aucun choix de couleur, ou quantité inférieure à 1 et supérieure à 100, popup alertant l'utilisateur de sélectionner</v>
+        <v>OK / Si aucun choix de couleur, ou quantité inférieure à 1 et supérieure à 100, popup alertant l'utilisateur d'indiquer sa sélection</v>
       </c>
     </row>
     <row r="6">
@@ -479,6 +491,9 @@
       <c r="B6" t="str">
         <v>Validation de l'article</v>
       </c>
+      <c r="C6" t="str">
+        <v>Envoie dans le Local Storage de la couleur et de la quantité</v>
+      </c>
       <c r="D6" t="str">
         <v>Bouton validant la sélection de l'article et proposant d'être mené vers le panier</v>
       </c>
@@ -493,8 +508,11 @@
       <c r="B7" t="str">
         <v>Affichage de la liste d'article sélectionné</v>
       </c>
+      <c r="C7" t="str">
+        <v>Récupération des données du Local Storage, et récupération de l'image dans le fichier JSON</v>
+      </c>
       <c r="D7" t="str">
-        <v>Récapitulatif de tous les articles sélectionnés avec son coloris, sa quantité, et son prix</v>
+        <v>Récapitulatif de tous les articles sélectionnés avec son coloris, sa quantité</v>
       </c>
       <c r="E7" t="str">
         <v>OK</v>
@@ -507,6 +525,9 @@
       <c r="B8" t="str">
         <v>Modificateur de quantité des articles</v>
       </c>
+      <c r="C8" t="str">
+        <v>Input numérique ajoutant ou diminuant la quantité dans le Local Storage</v>
+      </c>
       <c r="D8" t="str">
         <v>Nouveau champ numérique permettant de modifier la quantité préalablement sélectionnée</v>
       </c>
@@ -519,10 +540,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <v>Calcul du prix de l'article</v>
+        <v>Affichage du prix de l'article</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Récupération  du prix, ajouté dans le Local Storage</v>
       </c>
       <c r="D9" t="str">
-        <v>Le prix de l'article est affiché, en multipliant la quantité choisi</v>
+        <v>Le prix de l'article est affiché</v>
       </c>
       <c r="E9" t="str">
         <v>OK</v>
@@ -535,8 +559,11 @@
       <c r="B10" t="str">
         <v>Calcul du prix total de la commande</v>
       </c>
+      <c r="C10" t="str">
+        <v>Le prix total equivaut au à la somme de chaque articles multiplié par leur quantité</v>
+      </c>
       <c r="D10" t="str">
-        <v>Le total est affiché par l'addition de chaque article multiplié par sa quantité</v>
+        <v>Le total est affiché par l'addition de chaque article</v>
       </c>
       <c r="E10" t="str">
         <v>OK</v>
@@ -549,6 +576,9 @@
       <c r="B11" t="str">
         <v>Suppression d'un article choisi</v>
       </c>
+      <c r="C11" t="str">
+        <v>Bouton cliquable supprimant le produit du Local Storage</v>
+      </c>
       <c r="D11" t="str">
         <v>Un bouton de suppression cliquable enlevant du récapitulatif l'article non voulu</v>
       </c>
@@ -563,6 +593,9 @@
       <c r="B12" t="str">
         <v>Validation des champs de texte dans le formulaire</v>
       </c>
+      <c r="C12" t="str">
+        <v>REGEX, avec messages d'erreurs pour chaque champs</v>
+      </c>
       <c r="D12" t="str">
         <v>Champ de texte alpha/numérique, selon les champs sélectionnés</v>
       </c>
@@ -577,6 +610,9 @@
       <c r="B13" t="str">
         <v>Bouton de validation de la commande</v>
       </c>
+      <c r="C13" t="str">
+        <v>Bouton confirmant la validité du formulaire, et qui effectue une redirection de page</v>
+      </c>
       <c r="D13" t="str">
         <v>Bouton validant la commande cliquable, et redirige vers la page de confirmation</v>
       </c>
@@ -591,11 +627,14 @@
       <c r="B14" t="str">
         <v>Affichage du numéro de commande</v>
       </c>
+      <c r="C14" t="str">
+        <v>Récupération d'un numéro aléatoire de confirmation de commande du fichier JSON</v>
+      </c>
       <c r="D14" t="str">
         <v>Un numéro de commande s'affiche, liant les inscriptions du formulaire utilisateur, et son choix des articles</v>
       </c>
       <c r="E14" t="str">
-        <v>OK / Si l'on inscrit l'adresse intenret de la page commande, un champ de texte indiquant Undefined sera inscrit</v>
+        <v>OK / Si l'on inscrit l'adresse intenret de la page commande, la commande sera indiquée comme étant validée, sans numéro de commande inscrit</v>
       </c>
     </row>
   </sheetData>

</xml_diff>